<commit_message>
added regression tree model
</commit_message>
<xml_diff>
--- a/data/GitAndroidAnalysis/repo_analysis/emails.xlsx
+++ b/data/GitAndroidAnalysis/repo_analysis/emails.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E090A6A-75C4-4D9D-913D-5050585DF94D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8189CC70-596C-4128-8930-107929402A8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13137,8 +13137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1630"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1639" workbookViewId="0">
-      <selection activeCell="F1590" sqref="F1590"/>
+    <sheetView tabSelected="1" topLeftCell="A1609" workbookViewId="0">
+      <selection activeCell="C1612" sqref="C1612:C1618"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>